<commit_message>
batch allocation with id
</commit_message>
<xml_diff>
--- a/batch-group-allocation/TCS_Java Microservices_Project allocation_Batch 4.xlsx
+++ b/batch-group-allocation/TCS_Java Microservices_Project allocation_Batch 4.xlsx
@@ -10,9 +10,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$83</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="93">
   <si>
     <t>ID</t>
   </si>
@@ -297,6 +297,18 @@
   </si>
   <si>
     <t>Appala Edala Ravikiran</t>
+  </si>
+  <si>
+    <t>BATCH -ID</t>
+  </si>
+  <si>
+    <t>not active</t>
+  </si>
+  <si>
+    <t>sai bhavani naga Surya Teja</t>
+  </si>
+  <si>
+    <t>b4</t>
   </si>
 </sst>
 </file>
@@ -753,20 +765,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="3"/>
     <col min="2" max="2" width="36.28515625" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="14.85546875" style="3"/>
+    <col min="3" max="3" width="14.85546875" style="3"/>
+    <col min="4" max="4" width="30.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="14.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -776,8 +791,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -788,7 +806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -799,7 +817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -810,7 +828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -821,7 +839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -832,7 +850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -843,7 +861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -854,7 +872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -865,7 +883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -876,7 +894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -887,7 +905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -898,7 +916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -909,7 +927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -920,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -931,7 +949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1118,7 +1136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1129,7 +1147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1140,7 +1158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1151,7 +1169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1162,7 +1180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1173,7 +1191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1184,7 +1202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1195,7 +1213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1206,7 +1224,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1217,7 +1235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1228,7 +1246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1238,8 +1256,11 @@
       <c r="C43" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1250,7 +1271,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1261,7 +1282,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1272,7 +1293,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1283,7 +1304,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1293,8 +1314,11 @@
       <c r="C48" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1305,7 +1329,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1316,7 +1340,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1327,7 +1351,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1338,7 +1362,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1348,8 +1372,14 @@
       <c r="C53" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="3">
+        <v>103</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1360,7 +1390,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1371,7 +1401,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1382,7 +1412,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1393,7 +1423,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -1403,8 +1433,11 @@
       <c r="C58" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -1415,7 +1448,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -1426,7 +1459,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -1437,7 +1470,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -1448,7 +1481,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -1458,8 +1491,14 @@
       <c r="C63" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" s="3">
+        <v>105</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -1470,7 +1509,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1481,7 +1520,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -1492,7 +1531,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -1503,7 +1542,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -1513,8 +1552,11 @@
       <c r="C68" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -1525,7 +1567,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -1536,7 +1578,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -1547,7 +1589,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -1558,7 +1600,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -1568,8 +1610,11 @@
       <c r="C73" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -1580,7 +1625,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -1591,7 +1636,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -1602,56 +1647,68 @@
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>76</v>
-      </c>
-      <c r="B77" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D77" s="3">
+        <v>108</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
         <v>78</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
-        <v>77</v>
-      </c>
       <c r="B78" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
         <v>79</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
-        <v>78</v>
-      </c>
       <c r="B79" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
         <v>80</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
-        <v>79</v>
-      </c>
       <c r="B80" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>45</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>45</v>
@@ -1659,39 +1716,47 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B82" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
         <v>83</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
-        <v>82</v>
-      </c>
-      <c r="B83" s="11" t="s">
+      <c r="B83" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <v>83</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
         <v>84</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
-        <v>83</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>85</v>
+      <c r="B85" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C84">
+  <autoFilter ref="A1:C83">
     <filterColumn colId="2">
       <filters>
         <filter val="B4"/>

</xml_diff>